<commit_message>
Added test data to simple steel model
</commit_message>
<xml_diff>
--- a/data/steel/steel_WholeMill_var.xlsx
+++ b/data/steel/steel_WholeMill_var.xlsx
@@ -996,7 +996,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D16" sqref="D16"/>
+      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1969,7 +1969,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F13" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>